<commit_message>
first update in a while, updated TAB cover and requirements, version incremented to 7.16.1
</commit_message>
<xml_diff>
--- a/99 - End of Report/EndofReport/AAB-EndofReport.xlsx
+++ b/99 - End of Report/EndofReport/AAB-EndofReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Campos\ied-reports\report-builder-branches\report-builder\99 - End of Report\EndofReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B995CF-0013-444E-B3FC-067660FCE456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3053A315-D276-49A1-A864-FC856896E0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="6" xr2:uid="{B5AD7E83-9F06-4517-A043-647BDDAC5937}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="30960" windowHeight="12204" activeTab="6" xr2:uid="{A15E9BDA-2FB6-45E6-A874-7B698A32ED41}"/>
   </bookViews>
   <sheets>
     <sheet name="CALIBRFLYER" sheetId="2" r:id="rId1"/>
@@ -717,7 +717,7 @@
     <t>REMARKS</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>test</t>
   </si>
   <si>
     <t>Reduced Mechanical Drawings</t>
@@ -2038,9 +2038,9 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="3" xr:uid="{B198E28C-5452-448A-BA8C-A690448BA9C3}"/>
-    <cellStyle name="Normal 4" xfId="4" xr:uid="{190132B5-D614-4499-B989-5AB5FCFD2C90}"/>
-    <cellStyle name="Normal 9" xfId="2" xr:uid="{B1902674-F34E-4E5D-8005-9B57998DD67D}"/>
+    <cellStyle name="Normal 10" xfId="3" xr:uid="{0C8B54B3-F22A-44B1-AAEC-7F88A67C2F98}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{EC76F945-A590-496C-8F7B-CCFE9E848866}"/>
+    <cellStyle name="Normal 9" xfId="2" xr:uid="{F8851B10-0918-451D-B7BE-447D2F14B283}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
@@ -2091,7 +2091,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C600AD5-B114-4A0A-A342-F0BEE472C032}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{415B2C3C-D05A-4953-819D-37492E69720F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2146,7 +2146,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADB62EC8-CC9F-40BB-8BFB-178F6AFB6197}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F88C898-8950-49D4-8664-F2C722C05F06}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2201,7 +2201,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A062A71F-5D20-4CBE-8D5F-B8192A8E4A62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD89A0FD-1FC1-46E5-B34E-E4AE060808BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2256,7 +2256,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4B7E41-B88C-4B96-BEE5-4108EEA99289}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB754CE0-C9BA-4EFF-A7DE-5084760466AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2311,7 +2311,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7B1204C-5219-40F6-BA24-F817F3F59FD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD238CA7-556C-4D42-B923-89C72E39095E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2366,7 +2366,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E50470F-DA41-44BA-AF4E-A848D4481E0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A0F044C-9758-40DB-B783-2E91FCEE9B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2421,7 +2421,7 @@
         <xdr:cNvPr id="2" name="logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12C230B-382F-4E9E-9C41-DB500B89B5F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D4CDEFF-8308-4478-876F-133C25290355}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3772,7 +3772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BD377A-1EC6-491B-A7DB-BB304E7A0088}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F649BEF2-35C1-4AE3-91C8-D4C107698729}">
   <sheetPr codeName="Sheet58">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6229,7 +6229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A06A0D-B48F-4A26-BADC-38715D35E173}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD880F4A-651B-488F-B252-F1BD700D51EE}">
   <sheetPr codeName="Sheet25">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -10802,7 +10802,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A62" xr:uid="{88BE253E-9CA4-499C-9879-57F9663B4E53}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A60:A62" xr:uid="{5F911F46-41C7-4FDB-9AB8-5B4FE2471627}">
       <formula1>"GS"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10818,7 +10818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162A7D02-0E20-4230-97DA-27B442AFFD14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9680E32-FD30-467D-9086-F32BC354ECA8}">
   <sheetPr codeName="Sheet59">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -13275,7 +13275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54DF4F3-4BB4-4A76-A8AD-112E7C5D6E5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B1A800-EAE6-43D8-8828-93019EC26FB4}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -15730,7 +15730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E460283E-CF5D-4690-A3B8-1976F5DFA0B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF54AB1-94EF-4CD6-87A8-C3A8F3A69755}">
   <sheetPr codeName="Sheet60">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -18187,7 +18187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C73A9C-92DF-4842-9883-B34BC27C1348}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81312D4-8935-4438-8EF6-BC1E317BCDAA}">
   <sheetPr codeName="Sheet21">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -21226,7 +21226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C02445-2ECA-46A3-B151-4250005697A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1556EB2D-4B4B-475C-A8F7-5A8214B9320C}">
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>